<commit_message>
update dbo_species chara baltica
</commit_message>
<xml_diff>
--- a/nbs/files/lut/dbo_species_cleaned.xlsx
+++ b/nbs/files/lut/dbo_species_cleaned.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/franckalbinet/pro/IAEA/MARIS/marisco/nbs/files/lut/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72D0690C-8175-C146-A7F0-32691CBC38C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61406C46-9774-3E44-8BF0-FDACD7C220BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15624,8 +15624,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L1612"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+    <sheetView tabSelected="1" topLeftCell="D1593" workbookViewId="0">
+      <selection activeCell="C1609" sqref="C1609"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -15633,6 +15633,7 @@
     <col min="1" max="1" width="32.5" customWidth="1"/>
     <col min="2" max="2" width="25.1640625" customWidth="1"/>
     <col min="3" max="3" width="33.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.1640625" customWidth="1"/>
     <col min="7" max="7" width="58.83203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
   </cols>
@@ -76820,11 +76821,14 @@
       <c r="F1612" t="s">
         <v>4915</v>
       </c>
-      <c r="G1612" t="s">
+      <c r="G1612" s="1" t="s">
         <v>4916</v>
       </c>
       <c r="H1612" t="s">
         <v>16</v>
+      </c>
+      <c r="K1612">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -76833,6 +76837,7 @@
   </sortState>
   <hyperlinks>
     <hyperlink ref="G1611" r:id="rId1" xr:uid="{052B5849-DECC-6D4E-A301-DA38F0F80B37}"/>
+    <hyperlink ref="G1612" r:id="rId2" xr:uid="{4D38A5DF-7B95-974B-93EE-BC57518773C4}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>